<commit_message>
Added 1) Bills 2) Expenses Details sheet Modified 1) Planning sheet for Hrs Planned changed to 3 hrs per day
</commit_message>
<xml_diff>
--- a/Docs/Planing_Sheet_for_LiBaAs.xlsx
+++ b/Docs/Planing_Sheet_for_LiBaAs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E161CF32-173B-4B9B-BE5C-49F5158DB80E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04014D0-7B6D-44E3-B309-552DB6F90A8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F1FA08E3-3F40-4603-B771-C7A93B7165F6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -164,6 +164,23 @@
   <si>
     <t>Status
  in %</t>
+  </si>
+  <si>
+    <t>Keypad Libraries Tested: First Level Demo shown
+CAN analyser ordered: From DigiKey
+BMS Vendor from Pune  finalized : SSK</t>
+  </si>
+  <si>
+    <t>Cost per hr : 850 Rs</t>
+  </si>
+  <si>
+    <t>Total Engineering  Cost</t>
+  </si>
+  <si>
+    <t>Paid Amount</t>
+  </si>
+  <si>
+    <t>Balance</t>
   </si>
 </sst>
 </file>
@@ -193,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,23 +340,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,6 +369,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -359,15 +397,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -376,11 +405,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,723 +722,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814C8FB9-A7C6-494B-BA79-DF6435FDDBA2}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.28515625" customWidth="1"/>
     <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>44217</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15">
-        <v>4</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="27">
+        <v>100</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5">
+      <c r="B3" s="14"/>
+      <c r="C3" s="4">
         <v>44218</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="4">
         <v>44219</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
+      <c r="B5" s="14"/>
+      <c r="C5" s="4">
         <v>44220</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="7">
         <v>0</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
+      <c r="B6" s="14"/>
+      <c r="C6" s="4">
         <v>44221</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5">
+      <c r="B7" s="14"/>
+      <c r="C7" s="4">
         <v>44222</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="15">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
         <v>44223</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="15">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="14">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>44224</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="15">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="7">
+        <v>3</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5">
+      <c r="B10" s="14"/>
+      <c r="C10" s="4">
         <v>44225</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="15">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5">
+      <c r="B11" s="14"/>
+      <c r="C11" s="4">
         <v>44226</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5">
+      <c r="B12" s="14"/>
+      <c r="C12" s="4">
         <v>44227</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="7">
         <v>0</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5">
+      <c r="B13" s="14"/>
+      <c r="C13" s="4">
         <v>44228</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="15">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5">
+      <c r="B14" s="14"/>
+      <c r="C14" s="4">
         <v>44229</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="15">
-        <v>4</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5">
+      <c r="B15" s="14"/>
+      <c r="C15" s="4">
         <v>44230</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="15">
-        <v>4</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="14">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
         <v>44231</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="15">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4">
         <v>44232</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="15">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="E17" s="7">
+        <v>3</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5">
+      <c r="B18" s="14"/>
+      <c r="C18" s="4">
         <v>44233</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="7">
         <v>0</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5">
+      <c r="B19" s="14"/>
+      <c r="C19" s="4">
         <v>44234</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="7">
         <v>0</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5">
+      <c r="B20" s="14"/>
+      <c r="C20" s="4">
         <v>44235</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="15">
-        <v>4</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="7">
+        <v>3</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5">
+      <c r="B21" s="14"/>
+      <c r="C21" s="4">
         <v>44236</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="15">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="E21" s="7">
+        <v>3</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5">
+      <c r="B22" s="14"/>
+      <c r="C22" s="4">
         <v>44237</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14">
         <v>4</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>44238</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="15">
-        <v>4</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="E23" s="7">
+        <v>3</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5">
+      <c r="B24" s="14"/>
+      <c r="C24" s="4">
         <v>44239</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="15">
-        <v>4</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="E24" s="7">
+        <v>3</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5">
+      <c r="B25" s="14"/>
+      <c r="C25" s="4">
         <v>44240</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5">
+      <c r="B26" s="14"/>
+      <c r="C26" s="4">
         <v>44241</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="7">
         <v>0</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5">
+      <c r="B27" s="14"/>
+      <c r="C27" s="4">
         <v>44242</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="15">
-        <v>4</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="7">
+        <v>3</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="4">
         <v>44243</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="15">
-        <v>4</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="E28" s="7">
+        <v>3</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5">
+      <c r="B29" s="14"/>
+      <c r="C29" s="4">
         <v>44244</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="15">
-        <v>4</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="E29" s="7">
+        <v>3</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="14">
         <v>5</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>44245</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="15">
-        <v>4</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="E30" s="7">
+        <v>3</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5">
+      <c r="B31" s="14"/>
+      <c r="C31" s="4">
         <v>44246</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="15">
-        <v>4</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="E31" s="7">
+        <v>3</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5">
+      <c r="B32" s="14"/>
+      <c r="C32" s="4">
         <v>44247</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="7">
         <v>0</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5">
+      <c r="B33" s="14"/>
+      <c r="C33" s="4">
         <v>44248</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="7">
         <v>0</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="9" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="7">
         <f>SUM(E2:E33)</f>
-        <v>88</v>
-      </c>
-      <c r="F34" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="13"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="7">
+        <f>E34*850</f>
+        <v>56100</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="3">
+        <v>20000</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="3">
+        <f>E35-G35</f>
+        <v>36100</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="H6:H12"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I6:I12"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H13:H19"/>
+    <mergeCell ref="I13:I19"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H26"/>
+    <mergeCell ref="I20:I26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="B30:B33"/>
@@ -1422,34 +1507,7 @@
     <mergeCell ref="I27:I33"/>
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="G32:G33"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H26"/>
-    <mergeCell ref="I20:I26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H13:H19"/>
-    <mergeCell ref="I13:I19"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="H6:H12"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I6:I12"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
     <mergeCell ref="B23:B29"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="F20:F24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1459,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417F7FBA-7E36-4D3A-81C9-64BD87824939}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,31 +1535,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1509,109 +1567,109 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>44257</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3">
-        <v>4</v>
-      </c>
-      <c r="F2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5">
+      <c r="B3" s="14"/>
+      <c r="C3" s="4">
         <v>44258</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3">
-        <v>4</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
+      <c r="B4" s="14"/>
+      <c r="C4" s="4">
         <v>44259</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
+      <c r="B5" s="14"/>
+      <c r="C5" s="4">
         <v>44260</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="3">
-        <v>4</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
+      <c r="B6" s="14"/>
+      <c r="C6" s="4">
         <v>44261</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="3">
-        <v>4</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5">
+      <c r="B7" s="14"/>
+      <c r="C7" s="4">
         <v>44262</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1620,19 +1678,19 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
         <v>44263</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1641,118 +1699,118 @@
       <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="14">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>44264</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3">
-        <v>4</v>
-      </c>
-      <c r="F9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5">
+      <c r="B10" s="14"/>
+      <c r="C10" s="4">
         <v>44265</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="3">
-        <v>4</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5">
+      <c r="B11" s="14"/>
+      <c r="C11" s="4">
         <v>44266</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3">
-        <v>4</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5">
+      <c r="B12" s="14"/>
+      <c r="C12" s="4">
         <v>44267</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="3">
-        <v>4</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5">
+      <c r="B13" s="14"/>
+      <c r="C13" s="4">
         <v>44268</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="3">
-        <v>4</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5">
+      <c r="B14" s="14"/>
+      <c r="C14" s="4">
         <v>44269</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1761,19 +1819,19 @@
       <c r="E14" s="3">
         <v>0</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5">
+      <c r="B15" s="14"/>
+      <c r="C15" s="4">
         <v>44270</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1782,118 +1840,118 @@
       <c r="E15" s="3">
         <v>0</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="14">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
         <v>44271</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="3">
-        <v>4</v>
-      </c>
-      <c r="F16" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4">
         <v>44272</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3">
-        <v>4</v>
-      </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5">
+      <c r="B18" s="14"/>
+      <c r="C18" s="4">
         <v>44273</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="3">
-        <v>4</v>
-      </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5">
+      <c r="B19" s="14"/>
+      <c r="C19" s="4">
         <v>44274</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="3">
-        <v>4</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5">
+      <c r="B20" s="14"/>
+      <c r="C20" s="4">
         <v>44275</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="3">
-        <v>4</v>
-      </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5">
+      <c r="B21" s="14"/>
+      <c r="C21" s="4">
         <v>44276</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1902,19 +1960,19 @@
       <c r="E21" s="3">
         <v>0</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5">
+      <c r="B22" s="14"/>
+      <c r="C22" s="4">
         <v>44277</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1923,118 +1981,118 @@
       <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="14">
         <v>4</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>44278</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3">
-        <v>4</v>
-      </c>
-      <c r="F23" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5">
+      <c r="B24" s="14"/>
+      <c r="C24" s="4">
         <v>44279</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="3">
-        <v>4</v>
-      </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5">
+      <c r="B25" s="14"/>
+      <c r="C25" s="4">
         <v>44280</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="3">
-        <v>4</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5">
+      <c r="B26" s="14"/>
+      <c r="C26" s="4">
         <v>44281</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="3">
-        <v>4</v>
-      </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5">
+      <c r="B27" s="14"/>
+      <c r="C27" s="4">
         <v>44282</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3">
-        <v>4</v>
-      </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="4">
         <v>44283</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2043,19 +2101,19 @@
       <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5">
+      <c r="B29" s="14"/>
+      <c r="C29" s="4">
         <v>44284</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2064,54 +2122,61 @@
       <c r="E29" s="3">
         <v>0</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="9" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="3">
         <f>SUM(E2:E29)</f>
-        <v>80</v>
-      </c>
-      <c r="F30" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="13"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="7">
+        <f>E30*850</f>
+        <v>51000</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="3">
+        <f>E31-G31</f>
+        <v>51000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="H9:H15"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="H23:H29"/>
-    <mergeCell ref="I9:I15"/>
-    <mergeCell ref="I16:I22"/>
-    <mergeCell ref="I23:I29"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="G2:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H2:H8"/>
+  <mergeCells count="31">
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="I2:I8"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="F30:I30"/>
@@ -2121,6 +2186,27 @@
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="B16:B22"/>
     <mergeCell ref="B2:B8"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="H23:H29"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="I16:I22"/>
+    <mergeCell ref="I23:I29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Timesheet for Customer
</commit_message>
<xml_diff>
--- a/Docs/Planing_Sheet_for_LiBaAs.xlsx
+++ b/Docs/Planing_Sheet_for_LiBaAs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DECB1-4932-457D-B5B9-6239A8FD79B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2FA3D8-CB84-4F0D-B4D6-D41B699CC96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F1FA08E3-3F40-4603-B771-C7A93B7165F6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,47 @@
   <si>
     <t>RTOS Based Firmware designed for each mode and tested ADD_Credits and other logics like Charging/ Credits expired
 Design Layout activity on going waiting for component availability confirmation from vendor</t>
+  </si>
+  <si>
+    <t>Embedded system components ordered
+based on availability in local market
+Checking in local market took time</t>
+  </si>
+  <si>
+    <t>Worked on few issues of LCD
+ for printing on different lines
+Worked to generate simulated CAN data with CAN Analyzer and successfully receive it on the ES
+We were able to print this simulated CAN data</t>
+  </si>
+  <si>
+    <t>Tested Contactor circuitary
+Tested Dev board 
+integration with CAN libraries with BMS CAN data output</t>
+  </si>
+  <si>
+    <t>Code designed and tested
+for updation of parameters 
+Working as expected
+Layout designed</t>
+  </si>
+  <si>
+    <t>Integrateed both logics
+1. Tested all the data received updates parameter
+2. Tested if load disconnects after credits are overed.</t>
+  </si>
+  <si>
+    <t>1. Tested for half battery
+Capacity
+2. Tested for full battery charge
+3. Tested for small amount of credits left</t>
+  </si>
+  <si>
+    <t>Apart from above activities we have worked on packaging
+of the device to help customer showcase it better way</t>
+  </si>
+  <si>
+    <t>Battery pack delivered on 21-June-21 Due to heavy lockdown
+measures in Maharashtra</t>
   </si>
 </sst>
 </file>
@@ -340,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +404,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,27 +431,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,19 +450,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,9 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814C8FB9-A7C6-494B-BA79-DF6435FDDBA2}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,7 +836,7 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
       <c r="C2" s="4">
@@ -800,16 +848,16 @@
       <c r="E2" s="7">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="14">
         <v>100</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -817,7 +865,7 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4">
         <v>44218</v>
       </c>
@@ -827,16 +875,16 @@
       <c r="E3" s="7">
         <v>3</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4">
         <v>44219</v>
       </c>
@@ -846,18 +894,18 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="13"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4">
         <v>44220</v>
       </c>
@@ -867,16 +915,16 @@
       <c r="E5" s="7">
         <v>0</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="13"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4">
         <v>44221</v>
       </c>
@@ -886,16 +934,16 @@
       <c r="E6" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>100</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -903,7 +951,7 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4">
         <v>44222</v>
       </c>
@@ -913,16 +961,16 @@
       <c r="E7" s="7">
         <v>3</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4">
         <v>44223</v>
       </c>
@@ -932,16 +980,16 @@
       <c r="E8" s="7">
         <v>3</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
       <c r="C9" s="4">
@@ -953,16 +1001,16 @@
       <c r="E9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4">
         <v>44225</v>
       </c>
@@ -972,16 +1020,16 @@
       <c r="E10" s="7">
         <v>3</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4">
         <v>44226</v>
       </c>
@@ -991,18 +1039,18 @@
       <c r="E11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4">
         <v>44227</v>
       </c>
@@ -1012,16 +1060,16 @@
       <c r="E12" s="7">
         <v>0</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4">
         <v>44228</v>
       </c>
@@ -1031,16 +1079,16 @@
       <c r="E13" s="7">
         <v>3</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="29">
-        <v>80</v>
-      </c>
-      <c r="I13" s="28" t="s">
+      <c r="H13" s="14">
+        <v>100</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1048,7 +1096,7 @@
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4">
         <v>44229</v>
       </c>
@@ -1058,16 +1106,16 @@
       <c r="E14" s="7">
         <v>3</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="16"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4">
         <v>44230</v>
       </c>
@@ -1077,16 +1125,16 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="16"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
       <c r="C16" s="4">
@@ -1098,16 +1146,16 @@
       <c r="E16" s="7">
         <v>3</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="16"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4">
         <v>44232</v>
       </c>
@@ -1117,16 +1165,16 @@
       <c r="E17" s="7">
         <v>3</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="16"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4">
         <v>44233</v>
       </c>
@@ -1136,18 +1184,18 @@
       <c r="E18" s="7">
         <v>0</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="16"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4">
         <v>44234</v>
       </c>
@@ -1157,16 +1205,16 @@
       <c r="E19" s="7">
         <v>0</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="16"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="4">
         <v>44235</v>
       </c>
@@ -1176,20 +1224,24 @@
       <c r="E20" s="7">
         <v>3</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
+      <c r="H20" s="14">
+        <v>100</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4">
         <v>44236</v>
       </c>
@@ -1199,16 +1251,16 @@
       <c r="E21" s="7">
         <v>3</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="4">
         <v>44237</v>
       </c>
@@ -1218,16 +1270,16 @@
       <c r="E22" s="7">
         <v>3</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="11">
         <v>4</v>
       </c>
       <c r="C23" s="4">
@@ -1239,16 +1291,16 @@
       <c r="E23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="4">
         <v>44239</v>
       </c>
@@ -1258,16 +1310,16 @@
       <c r="E24" s="7">
         <v>3</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="4">
         <v>44240</v>
       </c>
@@ -1277,18 +1329,18 @@
       <c r="E25" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4">
         <v>44241</v>
       </c>
@@ -1298,16 +1350,16 @@
       <c r="E26" s="7">
         <v>0</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="4">
         <v>44242</v>
       </c>
@@ -1317,20 +1369,24 @@
       <c r="E27" s="7">
         <v>3</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="H27" s="14">
+        <v>100</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4">
         <v>44243</v>
       </c>
@@ -1340,16 +1396,16 @@
       <c r="E28" s="7">
         <v>3</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4">
         <v>44244</v>
       </c>
@@ -1359,16 +1415,16 @@
       <c r="E29" s="7">
         <v>3</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="11">
         <v>5</v>
       </c>
       <c r="C30" s="4">
@@ -1380,16 +1436,16 @@
       <c r="E30" s="7">
         <v>3</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4">
         <v>44246</v>
       </c>
@@ -1399,16 +1455,16 @@
       <c r="E31" s="7">
         <v>3</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4">
         <v>44247</v>
       </c>
@@ -1418,18 +1474,18 @@
       <c r="E32" s="7">
         <v>0</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4">
         <v>44248</v>
       </c>
@@ -1439,17 +1495,17 @@
       <c r="E33" s="7">
         <v>0</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
@@ -1457,19 +1513,19 @@
         <f>SUM(E2:E33)</f>
         <v>66</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="3" t="s">
         <v>38</v>
       </c>
@@ -1493,28 +1549,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="I27:I33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H26"/>
-    <mergeCell ref="I20:I26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H13:H19"/>
-    <mergeCell ref="I13:I19"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="H6:H12"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I6:I12"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F6:F10"/>
@@ -1531,6 +1565,28 @@
     <mergeCell ref="F27:F31"/>
     <mergeCell ref="G27:G31"/>
     <mergeCell ref="H27:H33"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="H6:H12"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I6:I12"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H13:H19"/>
+    <mergeCell ref="I13:I19"/>
+    <mergeCell ref="I27:I33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H26"/>
+    <mergeCell ref="I20:I26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1540,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417F7FBA-7E36-4D3A-81C9-64BD87824939}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,11 +1646,11 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>1</v>
       </c>
       <c r="C2" s="4">
-        <v>44257</v>
+        <v>44368</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1608,16 +1664,20 @@
       <c r="G2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="H2" s="28">
+        <v>100</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4">
-        <v>44258</v>
+        <v>44369</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -1625,18 +1685,18 @@
       <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="20"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4">
-        <v>44259</v>
+        <v>44370</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -1644,18 +1704,18 @@
       <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="20"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4">
-        <v>44260</v>
+        <v>44371</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
@@ -1663,18 +1723,18 @@
       <c r="E5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="20"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4">
-        <v>44261</v>
+        <v>44372</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -1682,18 +1742,18 @@
       <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="20"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4">
-        <v>44262</v>
+        <v>44373</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
@@ -1705,16 +1765,16 @@
         <v>28</v>
       </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4">
-        <v>44263</v>
+        <v>44374</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
@@ -1722,20 +1782,20 @@
       <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="21"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
       <c r="C9" s="4">
-        <v>44264</v>
+        <v>44375</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -1749,16 +1809,20 @@
       <c r="G9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="28">
+        <v>100</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4">
-        <v>44265</v>
+        <v>44376</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
@@ -1766,18 +1830,18 @@
       <c r="E10" s="3">
         <v>3</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="20"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="29"/>
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4">
-        <v>44266</v>
+        <v>44377</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
@@ -1785,18 +1849,18 @@
       <c r="E11" s="3">
         <v>3</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="20"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4">
-        <v>44267</v>
+        <v>44378</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>4</v>
@@ -1804,18 +1868,18 @@
       <c r="E12" s="3">
         <v>3</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="20"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="29"/>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4">
-        <v>44268</v>
+        <v>44379</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
@@ -1823,18 +1887,18 @@
       <c r="E13" s="3">
         <v>3</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="20"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4">
-        <v>44269</v>
+        <v>44380</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
@@ -1846,16 +1910,16 @@
         <v>28</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="20"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4">
-        <v>44270</v>
+        <v>44381</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1865,18 +1929,18 @@
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="21"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
       <c r="C16" s="4">
-        <v>44271</v>
+        <v>44382</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1890,16 +1954,20 @@
       <c r="G16" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="28">
+        <v>100</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4">
-        <v>44272</v>
+        <v>44383</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -1907,18 +1975,18 @@
       <c r="E17" s="3">
         <v>3</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="20"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4">
-        <v>44273</v>
+        <v>44384</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
@@ -1926,18 +1994,18 @@
       <c r="E18" s="3">
         <v>3</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="20"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="29"/>
       <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4">
-        <v>44274</v>
+        <v>44385</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>4</v>
@@ -1945,18 +2013,18 @@
       <c r="E19" s="3">
         <v>3</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="20"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="29"/>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="4">
-        <v>44275</v>
+        <v>44386</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
@@ -1966,16 +2034,16 @@
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
-      <c r="H20" s="20"/>
+      <c r="H20" s="29"/>
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4">
-        <v>44276</v>
+        <v>44387</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
@@ -1987,16 +2055,16 @@
         <v>28</v>
       </c>
       <c r="G21" s="22"/>
-      <c r="H21" s="20"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="4">
-        <v>44277</v>
+        <v>44388</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -2006,18 +2074,18 @@
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
-      <c r="H22" s="21"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="11">
         <v>4</v>
       </c>
       <c r="C23" s="4">
-        <v>44278</v>
+        <v>44389</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
@@ -2031,16 +2099,20 @@
       <c r="G23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="H23" s="28">
+        <v>100</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="4">
-        <v>44279</v>
+        <v>44390</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
@@ -2048,18 +2120,18 @@
       <c r="E24" s="3">
         <v>3</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="20"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="29"/>
       <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="4">
-        <v>44280</v>
+        <v>44391</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>10</v>
@@ -2067,18 +2139,18 @@
       <c r="E25" s="3">
         <v>3</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="20"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4">
-        <v>44281</v>
+        <v>44392</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
@@ -2086,18 +2158,18 @@
       <c r="E26" s="3">
         <v>3</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="4">
-        <v>44282</v>
+        <v>44393</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
@@ -2107,16 +2179,16 @@
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
-      <c r="H27" s="20"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4">
-        <v>44283</v>
+        <v>44394</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
@@ -2128,16 +2200,16 @@
         <v>28</v>
       </c>
       <c r="G28" s="22"/>
-      <c r="H28" s="20"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4">
-        <v>44284</v>
+        <v>44395</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>7</v>
@@ -2147,15 +2219,15 @@
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
-      <c r="H29" s="21"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="5" t="s">
         <v>23</v>
       </c>
@@ -2163,19 +2235,19 @@
         <f>SUM(E2:E29)</f>
         <v>60</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="3" t="s">
         <v>38</v>
       </c>
@@ -2197,23 +2269,18 @@
         <v>51000</v>
       </c>
     </row>
+    <row r="33" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F33" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F34" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H9:H15"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="H23:H29"/>
-    <mergeCell ref="I9:I15"/>
-    <mergeCell ref="I16:I22"/>
-    <mergeCell ref="I23:I29"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F27"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="I2:I8"/>
     <mergeCell ref="A30:C30"/>
@@ -2230,6 +2297,21 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H2:H8"/>
     <mergeCell ref="G9:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="H23:H29"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="I16:I22"/>
+    <mergeCell ref="I23:I29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>